<commit_message>
update uncertainty project group asignation for surgeries
</commit_message>
<xml_diff>
--- a/data/echoMRI/kotz04072025.xlsx
+++ b/data/echoMRI/kotz04072025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carosandovalcab/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carosandovalcaballero/Documents/GitHub/data/data/echoMRI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0739F9C-83D2-2040-BFD4-E09CE592BBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB53ED89-520B-C145-8A89-2304DBC2D969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="44800" windowHeight="25200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtractedScans" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>RecNumber</t>
   </si>
@@ -55,85 +55,52 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>2001</t>
-  </si>
-  <si>
-    <t>6176</t>
-  </si>
-  <si>
-    <t>6174</t>
-  </si>
-  <si>
-    <t>6189</t>
-  </si>
-  <si>
-    <t>2002</t>
-  </si>
-  <si>
-    <t>1003</t>
-  </si>
-  <si>
-    <t>6185</t>
-  </si>
-  <si>
-    <t>6177</t>
-  </si>
-  <si>
-    <t>6180</t>
-  </si>
-  <si>
-    <t>1002</t>
-  </si>
-  <si>
-    <t>1001</t>
-  </si>
-  <si>
-    <t>12:14:41 Apr 7; 2025; 27; ems</t>
-  </si>
-  <si>
-    <t>12:16:05 Apr 7; 2025; 27; ems</t>
-  </si>
-  <si>
-    <t>12:17:27 Apr 7; 2025; 27; ems</t>
-  </si>
-  <si>
-    <t>12:18:48 Apr 7; 2025; 32; ems</t>
-  </si>
-  <si>
-    <t>12:19:55 Apr 7; 2025; 31; ems</t>
-  </si>
-  <si>
-    <t>12:21:14 Apr 7; 2025; 27; ems</t>
-  </si>
-  <si>
-    <t>12:22:26 Apr 7; 2025; 31; ems</t>
-  </si>
-  <si>
-    <t>12:23:59 Apr 7; 2025; 31; ems</t>
-  </si>
-  <si>
-    <t>12:25:24 Apr 7; 2025; 36; ems</t>
-  </si>
-  <si>
-    <t>12:26:41 Apr 7; 2025; 27; ems</t>
-  </si>
-  <si>
-    <t>12:27:46 Apr 7; 2025; 31; ems</t>
-  </si>
-  <si>
-    <t>12:28:55 Apr 7; 2025; 32; ems</t>
-  </si>
-  <si>
-    <t>12:30:01 Apr 7; 2025; 31; ems</t>
-  </si>
-  <si>
-    <t>12:37:02 Apr 7; 2025; 32; ems</t>
-  </si>
-  <si>
-    <t>12:38:23 Apr 7; 2025; 31; ems</t>
-  </si>
-  <si>
-    <t>12:39:30 Apr 7; 2025; 31; ems</t>
+    <t>12:14:41 Apr 7, 2025; 27; ems</t>
+  </si>
+  <si>
+    <t>12:16:05 Apr 7, 2025; 27; ems</t>
+  </si>
+  <si>
+    <t>12:17:27 Apr 7, 2025; 27; ems</t>
+  </si>
+  <si>
+    <t>12:18:48 Apr 7, 2025; 32; ems</t>
+  </si>
+  <si>
+    <t>12:19:55 Apr 7, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>12:21:14 Apr 7, 2025; 27; ems</t>
+  </si>
+  <si>
+    <t>12:22:26 Apr 7, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>12:23:59 Apr 7, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>12:25:24 Apr 7, 2025; 36; ems</t>
+  </si>
+  <si>
+    <t>12:26:41 Apr 7, 2025; 27; ems</t>
+  </si>
+  <si>
+    <t>12:27:46 Apr 7, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>12:28:55 Apr 7, 2025; 32; ems</t>
+  </si>
+  <si>
+    <t>12:30:01 Apr 7, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>12:37:02 Apr 7, 2025; 32; ems</t>
+  </si>
+  <si>
+    <t>12:38:23 Apr 7, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>12:39:30 Apr 7, 2025; 31; ems</t>
   </si>
 </sst>
 </file>
@@ -474,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -535,7 +502,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -564,7 +531,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -593,7 +560,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -622,7 +589,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -651,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -664,8 +631,8 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
+      <c r="B7">
+        <v>313</v>
       </c>
       <c r="C7">
         <v>3.24</v>
@@ -680,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -693,8 +660,8 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>11</v>
+      <c r="B8">
+        <v>318</v>
       </c>
       <c r="C8">
         <v>8.06</v>
@@ -709,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -722,8 +689,8 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>12</v>
+      <c r="B9">
+        <v>316</v>
       </c>
       <c r="C9">
         <v>4.82</v>
@@ -738,7 +705,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -751,8 +718,8 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>13</v>
+      <c r="B10">
+        <v>327</v>
       </c>
       <c r="C10">
         <v>2.64</v>
@@ -767,7 +734,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -780,8 +747,8 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>14</v>
+      <c r="B11">
+        <v>315</v>
       </c>
       <c r="C11">
         <v>15.7</v>
@@ -796,7 +763,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -809,8 +776,8 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>15</v>
+      <c r="B12">
+        <v>311</v>
       </c>
       <c r="C12">
         <v>6.48</v>
@@ -825,7 +792,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -838,8 +805,8 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>16</v>
+      <c r="B13">
+        <v>300</v>
       </c>
       <c r="C13">
         <v>5.73</v>
@@ -854,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -867,8 +834,8 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>17</v>
+      <c r="B14">
+        <v>320</v>
       </c>
       <c r="C14">
         <v>9.8699999999999992</v>
@@ -883,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -896,8 +863,8 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>18</v>
+      <c r="B15">
+        <v>324</v>
       </c>
       <c r="C15">
         <v>8.1300000000000008</v>
@@ -912,7 +879,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -925,8 +892,8 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>19</v>
+      <c r="B16">
+        <v>299</v>
       </c>
       <c r="C16">
         <v>7.2</v>
@@ -941,7 +908,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -954,8 +921,8 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>20</v>
+      <c r="B17">
+        <v>326</v>
       </c>
       <c r="C17">
         <v>6.27</v>
@@ -970,7 +937,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="H17">
         <v>1</v>

</xml_diff>